<commit_message>
Documents Converted to PDFs, updated links where appropriate
</commit_message>
<xml_diff>
--- a/Current_Status/Project_Schedule.xlsx
+++ b/Current_Status/Project_Schedule.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\2017\Semester 2 2017\4221\Schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\GuidestarLaser\Current_Status\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Involve Celine</t>
   </si>
@@ -92,6 +92,30 @@
   <si>
     <t>Project Showcase</t>
   </si>
+  <si>
+    <t>Complete Work Package Reports</t>
+  </si>
+  <si>
+    <t>Finalise CoDR and Handover</t>
+  </si>
+  <si>
+    <t>Vendor Meeting, Client Meeting</t>
+  </si>
+  <si>
+    <t>No Client Meeting</t>
+  </si>
+  <si>
+    <t>Client Meeting</t>
+  </si>
+  <si>
+    <t>Client Meeting, Complete Ph1</t>
+  </si>
+  <si>
+    <t>No Client Meeting, Compelte Ph2, Vibration Measurements</t>
+  </si>
+  <si>
+    <t>Client Meeting, Cable Routing Measurements</t>
+  </si>
 </sst>
 </file>
 
@@ -100,15 +124,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\ mmm"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -162,8 +189,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,12 +220,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D2E9"/>
         <bgColor rgb="FFD9D2E9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA4C2F4"/>
-        <bgColor rgb="FFA4C2F4"/>
       </patternFill>
     </fill>
     <fill>
@@ -229,6 +257,17 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -239,54 +278,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -296,23 +337,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="4" builtinId="33"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="2" builtinId="11"/>
@@ -629,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -649,7 +698,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -717,7 +766,7 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="27" t="s">
         <v>13</v>
       </c>
     </row>
@@ -864,8 +913,11 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
+      <c r="F15" s="29" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
@@ -903,9 +955,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="E18" s="10"/>
+      <c r="F18" s="29" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
@@ -943,8 +998,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
+      <c r="F21" s="29" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
@@ -984,13 +1042,15 @@
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="F24" s="30" t="s">
+        <v>31</v>
+      </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
     </row>
@@ -1032,13 +1092,15 @@
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+      <c r="F27" s="31" t="s">
+        <v>28</v>
+      </c>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
     </row>
@@ -1078,8 +1140,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
+      <c r="F30" s="29" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
@@ -1114,10 +1179,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="17"/>
       <c r="E33" s="10"/>
+      <c r="F33" s="29" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
@@ -1152,9 +1220,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="10"/>
+      <c r="F36" s="30" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
@@ -1182,21 +1253,23 @@
         <v>43023</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17"/>
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E38" s="27" t="s">
+      <c r="E38" s="33" t="s">
         <v>23</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
-      <c r="B39" s="10"/>
+      <c r="B39" s="32" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
@@ -1224,15 +1297,18 @@
         <v>43030</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="25" t="s">
         <v>21</v>
       </c>
       <c r="E41" s="17"/>
     </row>
-    <row r="42" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="17"/>
+      <c r="F42" s="32" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="43" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="6">

</xml_diff>